<commit_message>
Update Dashboard - Scrum - Sprints 4 e 5.xlsx
</commit_message>
<xml_diff>
--- a/Documentação/Sprint 5/Dashboard - Scrum - Sprints 4 e 5.xlsx
+++ b/Documentação/Sprint 5/Dashboard - Scrum - Sprints 4 e 5.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23916"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71508FA7-FF5F-403C-A6C6-A9EECA699D58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E36335AF-BF62-4BF7-9A96-2AB22FD4E84A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,11 +15,11 @@
   <definedNames>
     <definedName name="Atividade">DadosDoRoteiro[Marco ou Atividade]</definedName>
     <definedName name="Meta">DadosDoRoteiro[Meta]</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Dados do Roteiro'!$1:$2</definedName>
     <definedName name="Prioridade">DadosDoRoteiro[Prioridade]</definedName>
     <definedName name="Resultado">DadosDoRoteiro[Resultado]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Dados do Roteiro'!$1:$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,12 +38,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Crie um Roteiro Ágil inserindo marcos ou atividades importantes na tabela Dados do Roteiro nesta planilha.
 O título desta planilha está na célula B1. 
 As informações sobre como usar esta planilha, incluindo instruções para leitores de tela, estão na planilha Sobre.
 Continue navegando pela coluna A para conferir mais instruções.</t>
+  </si>
+  <si>
+    <t>Dados da Linha do Tempo Ágil</t>
   </si>
   <si>
     <t xml:space="preserve">Os títulos da tabela estão nas células B2 a E2. Use filtros de cabeçalho para classificar a tabela e encontrar itens específicos.
@@ -54,46 +57,106 @@
 </t>
   </si>
   <si>
-    <t>Dados da Linha do Tempo Ágil</t>
-  </si>
-  <si>
     <t>Meta</t>
   </si>
   <si>
+    <t>Marco ou Atividade</t>
+  </si>
+  <si>
+    <t>Prioridade</t>
+  </si>
+  <si>
+    <t>Tarefa</t>
+  </si>
+  <si>
+    <t>Atribuído a</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>&lt;-- classificar tabela por Prioridade e Marco ou Atividade, em ordem crescente</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>Implementação de Strategy para Seriação Manual e Opcional e Atualização das Cenas e Controllers (16/03 e 17/03)</t>
+  </si>
+  <si>
+    <t>Caroline</t>
+  </si>
+  <si>
+    <t>1 – Alto</t>
+  </si>
+  <si>
+    <t>UC13 - Interface Gráfica - cena resultado Freelancer (15/03)</t>
+  </si>
+  <si>
+    <t>UC13 - Interface Gráfica - cena Consulta Colaborador e Gestor  + Implementação Java (17/03 e 18/03)</t>
+  </si>
+  <si>
     <t>Atual</t>
   </si>
   <si>
-    <t>Curto Prazo</t>
-  </si>
-  <si>
-    <t>Futuro</t>
-  </si>
-  <si>
-    <t>Concluído</t>
+    <t>UC13 - Interface Gráfica -Tabelas Colaborador e Gestor e Implementação Java  (17/03 e 18/03)</t>
+  </si>
+  <si>
+    <t>2 – Médio</t>
+  </si>
+  <si>
+    <t>UC13 - Documentação (15/03)</t>
+  </si>
+  <si>
+    <t>Bárbara, Caroline</t>
+  </si>
+  <si>
+    <t>UC13 - Implementação Java (19/03 e 20/03)</t>
+  </si>
+  <si>
+    <t>Correções no Restful API (15/03)</t>
+  </si>
+  <si>
+    <t>Bárbara</t>
+  </si>
+  <si>
+    <t>Correções no UC10A (15/03)</t>
+  </si>
+  <si>
+    <t>Scrum Sprint 5</t>
+  </si>
+  <si>
+    <t>Documentação UC13 (20/03)</t>
+  </si>
+  <si>
+    <t>DTOs (16/03-20/03)</t>
+  </si>
+  <si>
+    <t>Pequenos fixes (20/03)</t>
+  </si>
+  <si>
+    <t>BD - UC13 (21/03)</t>
+  </si>
+  <si>
+    <t>Relatório Análise, Design e Interfaces</t>
+  </si>
+  <si>
+    <t>Marta</t>
+  </si>
+  <si>
+    <t>Implementação de identificação de emails nas scenes FXML</t>
   </si>
   <si>
     <t>Adicione novos itens, inserindo novas linhas acima desta linha.</t>
-  </si>
-  <si>
-    <t>Marco ou Atividade</t>
-  </si>
-  <si>
-    <t>Prioridade</t>
-  </si>
-  <si>
-    <t>1 – Alto</t>
-  </si>
-  <si>
-    <t>Resultado</t>
-  </si>
-  <si>
-    <t>&lt;-- classificar tabela por Prioridade e Marco ou Atividade, em ordem crescente</t>
   </si>
   <si>
     <t>Há um Roteiro Ágil exibindo marcos e atividades da planilha Dados do Roteiro nesta planilha. 
 O título está na célula B1. 
 Os resultados com a frase "Sem Alteração" estão realçados em laranja claro, rgb(255, 230, 210).
 Marcos ou atividades concluídas estão realçados em verde claro, rgb(237, 251, 219).</t>
+  </si>
+  <si>
+    <t>Roteiro Ágil</t>
   </si>
   <si>
     <t>Os títulos do gráfico estão nas células B2, D2, F2 e H2. São eles: Concluído, Atual, Curto Prazo e Futuro. Modifique esses títulos para alterar os valores de seleção de Destino na tabela Dados do Roteiro na planilha Dados do Roteiro.
@@ -103,7 +166,10 @@
 Esta é a última instrução nesta planilha.</t>
   </si>
   <si>
-    <t>Roteiro Ágil</t>
+    <t>Curto Prazo</t>
+  </si>
+  <si>
+    <t>Futuro</t>
   </si>
   <si>
     <t>Sobre esta pasta de trabalho</t>
@@ -128,75 +194,18 @@
   <si>
     <t>Esta é a última instrução nesta planilha.</t>
   </si>
-  <si>
-    <t>Tarefa</t>
-  </si>
-  <si>
-    <t>Atribuído a</t>
-  </si>
-  <si>
-    <t>Caroline</t>
-  </si>
-  <si>
-    <t>Bárbara</t>
-  </si>
-  <si>
-    <t>UC13 - Interface Gráfica - cena resultado Freelancer (15/03)</t>
-  </si>
-  <si>
-    <t>Correções no Restful API (15/03)</t>
-  </si>
-  <si>
-    <t>Correções no UC10A (15/03)</t>
-  </si>
-  <si>
-    <t>2 – Médio</t>
-  </si>
-  <si>
-    <t>UC13 - Documentação (15/03)</t>
-  </si>
-  <si>
-    <t>Scrum Sprint 5</t>
-  </si>
-  <si>
-    <t>Bárbara, Caroline</t>
-  </si>
-  <si>
-    <t>UC13 - Interface Gráfica - cena Consulta Colaborador e Gestor  + Implementação Java (17/03 e 18/03)</t>
-  </si>
-  <si>
-    <t>UC13 - Interface Gráfica -Tabelas Colaborador e Gestor e Implementação Java  (17/03 e 18/03)</t>
-  </si>
-  <si>
-    <t>Implementação de Strategy para Seriação Manual e Opcional e Atualização das Cenas e Controllers (16/03 e 17/03)</t>
-  </si>
-  <si>
-    <t>UC13 - Implementação Java (19/03 e 20/03)</t>
-  </si>
-  <si>
-    <t>DTOs (16/03-20/03)</t>
-  </si>
-  <si>
-    <t>Pequenos fixes (20/03)</t>
-  </si>
-  <si>
-    <t>BD - UC13 (21/03)</t>
-  </si>
-  <si>
-    <t>Documentação UC13 (20/03)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,10 +705,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -780,9 +789,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="47" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -795,56 +801,59 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="48">
-    <cellStyle name="20% - Cor1" xfId="24" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Cor2" xfId="28" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Cor3" xfId="32" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Cor4" xfId="36" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Cor5" xfId="40" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Cor6" xfId="44" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Cor1" xfId="25" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Cor2" xfId="29" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Cor3" xfId="33" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Cor4" xfId="37" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Cor5" xfId="41" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Cor6" xfId="45" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Cor1" xfId="26" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Cor2" xfId="30" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Cor3" xfId="34" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Cor4" xfId="38" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Cor5" xfId="42" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Cor6" xfId="46" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="16" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula Ligada" xfId="17" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Cor1" xfId="23" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Cor2" xfId="27" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Cor3" xfId="31" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Cor4" xfId="35" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Cor5" xfId="39" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Cor6" xfId="43" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Correto" xfId="11" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="14" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="12" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Moeda" xfId="8" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Moeda [0]" xfId="9" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Neutro" xfId="13" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="24" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="28" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="32" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="36" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="40" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="44" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="25" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="29" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="33" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="37" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="41" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="45" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="26" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="30" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="34" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="38" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="42" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="46" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="23" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="27" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="31" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="35" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="39" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="43" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="12" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="18" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="6" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="7" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="8" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="9" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="21" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="11" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="14" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="17" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="13" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="47" xr:uid="{4459719E-C63E-4F79-8431-702264412897}"/>
-    <cellStyle name="Nota" xfId="20" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Percentagem" xfId="10" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Saída" xfId="15" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Separador de milhares [0]" xfId="7" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Texto de Aviso" xfId="19" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="21" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="20" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="15" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="10" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="22" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Verificar Célula" xfId="18" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Vírgula" xfId="6" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="19" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="16">
     <dxf>
@@ -1664,11 +1673,11 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.625" style="7" customWidth="1"/>
     <col min="2" max="2" width="15.625" customWidth="1"/>
@@ -1679,272 +1688,286 @@
     <col min="7" max="7" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="50.1" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="7" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="75">
+      <c r="B3" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>Implementação de Strategy para Seriação Manual e Opcional e Atualização das Cenas e Controllers (16/03 e 17/03) - Responsável: Caroline</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>UC13 - Interface Gráfica - cena resultado Freelancer (15/03) - Responsável: Caroline</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v xml:space="preserve">UC13 - Interface Gráfica - cena Consulta Colaborador e Gestor  + Implementação Java (17/03 e 18/03) - Responsável: </v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="60">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C6" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v xml:space="preserve">UC13 - Interface Gráfica -Tabelas Colaborador e Gestor e Implementação Java  (17/03 e 18/03) - Responsável: </v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C7" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>UC13 - Documentação (15/03) - Responsável: Bárbara, Caroline</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30">
       <c r="B8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C8" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>UC13 - Implementação Java (19/03 e 20/03) - Responsável: Caroline</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>Correções no Restful API (15/03) - Responsável: Bárbara</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30">
       <c r="B10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>Correções no UC10A (15/03) - Responsável: Caroline</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
       <c r="B11" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C11" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>Scrum Sprint 5 - Responsável: Caroline</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30">
       <c r="B12" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C12" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>Documentação UC13 (20/03) - Responsável: Bárbara</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30">
       <c r="B13" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C13" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>DTOs (16/03-20/03) - Responsável: Bárbara</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30">
       <c r="B14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>Pequenos fixes (20/03) - Responsável: Bárbara</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30">
       <c r="B15" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C15" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v>BD - UC13 (21/03) - Responsável: Bárbara</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="31.5" customHeight="1">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
       <c r="C16" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
-        <v xml:space="preserve"> - Responsável: </v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <v>Relatório Análise, Design e Interfaces - Responsável: Marta</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="44.25" customHeight="1">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
       <c r="C17" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
-        <v xml:space="preserve"> - Responsável: </v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+        <v>Implementação de identificação de emails nas scenes FXML - Responsável: Marta</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
       <c r="C18" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v xml:space="preserve"> - Responsável: </v>
@@ -1952,7 +1975,7 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6">
       <c r="C19" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v xml:space="preserve"> - Responsável: </v>
@@ -1960,7 +1983,7 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="C20" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v xml:space="preserve"> - Responsável: </v>
@@ -1968,7 +1991,7 @@
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="C21" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v xml:space="preserve"> - Responsável: </v>
@@ -1976,7 +1999,7 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="C22" t="str">
         <f>CONCATENATE(DadosDoRoteiro[[#This Row],[Tarefa]]," - Responsável: ", DadosDoRoteiro[[#This Row],[Atribuído a]])</f>
         <v xml:space="preserve"> - Responsável: </v>
@@ -1984,13 +2007,13 @@
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+    <row r="23" spans="2:6">
+      <c r="B23" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2023,14 +2046,14 @@
   </sheetPr>
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="30.625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="30.625" style="17" customWidth="1"/>
     <col min="3" max="3" width="6.625" style="3" customWidth="1"/>
     <col min="4" max="4" width="30.625" style="3" customWidth="1"/>
     <col min="5" max="5" width="6.625" style="3" customWidth="1"/>
@@ -2041,12 +2064,12 @@
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="50.1" customHeight="1" thickBot="1">
       <c r="A1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>16</v>
+        <v>34</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -2054,28 +2077,28 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:9" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="45" customHeight="1" thickTop="1">
       <c r="A2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>7</v>
+        <v>36</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="str">
+    <row r="3" spans="1:9" ht="75">
+      <c r="B3" s="16" t="str">
         <f t="array" ref="B3">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B3)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B3))))&amp;CHAR(10),"")</f>
         <v xml:space="preserve">Implementação de Strategy para Seriação Manual e Opcional e Atualização das Cenas e Controllers (16/03 e 17/03) - Responsável: Caroline 
 </v>
@@ -2097,8 +2120,8 @@
       </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="str">
+    <row r="4" spans="1:9" ht="75">
+      <c r="B4" s="16" t="str">
         <f t="array" ref="B4">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B4)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B4))))&amp;CHAR(10),"")</f>
         <v xml:space="preserve">UC13 - Interface Gráfica - cena resultado Freelancer (15/03) - Responsável: Caroline 
 </v>
@@ -2120,8 +2143,8 @@
       </c>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="str">
+    <row r="5" spans="1:9" ht="75">
+      <c r="B5" s="16" t="str">
         <f t="array" ref="B5">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B5)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B5))))&amp;CHAR(10),"")</f>
         <v xml:space="preserve">UC13 - Interface Gráfica - cena Consulta Colaborador e Gestor  + Implementação Java (17/03 e 18/03) - Responsável:  
 </v>
@@ -2143,8 +2166,8 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="str">
+    <row r="6" spans="1:9" ht="60">
+      <c r="B6" s="16" t="str">
         <f t="array" ref="B6">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B6)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B6))))&amp;CHAR(10),"")</f>
         <v xml:space="preserve">Correções no Restful API (15/03) - Responsável: Bárbara 
 </v>
@@ -2166,8 +2189,8 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="str">
+    <row r="7" spans="1:9" ht="75">
+      <c r="B7" s="16" t="str">
         <f t="array" ref="B7">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B7)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B7))))&amp;CHAR(10),"")</f>
         <v xml:space="preserve">Correções no UC10A (15/03) - Responsável: Caroline 
 </v>
@@ -2189,8 +2212,8 @@
       </c>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="str">
+    <row r="8" spans="1:9" ht="90">
+      <c r="B8" s="16" t="str">
         <f t="array" ref="B8">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B8)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B8))))&amp;CHAR(10),"")</f>
         <v xml:space="preserve">DTOs (16/03-20/03) - Responsável: Bárbara 
 </v>
@@ -2212,8 +2235,8 @@
       </c>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="str">
+    <row r="9" spans="1:9" ht="90">
+      <c r="B9" s="16" t="str">
         <f t="array" ref="B9">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B9)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B9))))&amp;CHAR(10),"")</f>
         <v xml:space="preserve">Pequenos fixes (20/03) - Responsável: Bárbara 
 </v>
@@ -2234,10 +2257,11 @@
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="str">
+    <row r="10" spans="1:9" ht="75">
+      <c r="B10" s="16" t="str">
         <f t="array" ref="B10">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B10)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B10))))&amp;CHAR(10),"")</f>
-        <v/>
+        <v xml:space="preserve">Relatório Análise, Design e Interfaces - Responsável: Marta 
+</v>
       </c>
       <c r="D10" s="5" t="str">
         <f t="array" ref="D10">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$D$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B10)))&amp;CHAR(10),"")</f>
@@ -2255,10 +2279,11 @@
       </c>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="str">
+    <row r="11" spans="1:9" ht="75">
+      <c r="B11" s="16" t="str">
         <f t="array" ref="B11">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B11)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B11))))&amp;CHAR(10),"")</f>
-        <v/>
+        <v xml:space="preserve">Implementação de identificação de emails nas scenes FXML - Responsável: Marta 
+</v>
       </c>
       <c r="D11" s="5" t="str">
         <f t="array" ref="D11">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$D$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B11)))&amp;CHAR(10),"")</f>
@@ -2276,8 +2301,8 @@
       </c>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="str">
+    <row r="12" spans="1:9" ht="60">
+      <c r="B12" s="16" t="str">
         <f t="array" ref="B12">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B12)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B12))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2297,8 +2322,8 @@
       </c>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="str">
+    <row r="13" spans="1:9" ht="60">
+      <c r="B13" s="16" t="str">
         <f t="array" ref="B13">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B13)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B13))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2318,8 +2343,8 @@
       </c>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="str">
+    <row r="14" spans="1:9" ht="45">
+      <c r="B14" s="16" t="str">
         <f t="array" ref="B14">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B14)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B14))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2339,8 +2364,8 @@
       </c>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="17" t="str">
+    <row r="15" spans="1:9" ht="60">
+      <c r="B15" s="16" t="str">
         <f t="array" ref="B15">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B15)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B15))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2360,8 +2385,8 @@
       </c>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B16" s="17" t="str">
+    <row r="16" spans="1:9" ht="60">
+      <c r="B16" s="16" t="str">
         <f t="array" ref="B16">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B16)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B16))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2381,8 +2406,8 @@
       </c>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="str">
+    <row r="17" spans="1:9" ht="60">
+      <c r="B17" s="16" t="str">
         <f t="array" ref="B17">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B17)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B17))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2402,8 +2427,8 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="str">
+    <row r="18" spans="1:9" ht="60">
+      <c r="B18" s="16" t="str">
         <f t="array" ref="B18">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B18)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B18))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2423,8 +2448,8 @@
       </c>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B19" s="17" t="str">
+    <row r="19" spans="1:9" ht="60">
+      <c r="B19" s="16" t="str">
         <f t="array" ref="B19">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B19)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B19))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2444,8 +2469,8 @@
       </c>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B20" s="17" t="str">
+    <row r="20" spans="1:9" ht="60">
+      <c r="B20" s="16" t="str">
         <f t="array" ref="B20">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B20)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B20))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2465,9 +2490,9 @@
       </c>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="60">
       <c r="A21" s="3"/>
-      <c r="B21" s="17" t="str">
+      <c r="B21" s="16" t="str">
         <f t="array" ref="B21">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B21)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B21))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2484,8 +2509,8 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B22" s="17" t="str">
+    <row r="22" spans="1:9" ht="60">
+      <c r="B22" s="16" t="str">
         <f t="array" ref="B22">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B22)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B22))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2502,8 +2527,8 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="str">
+    <row r="23" spans="1:9" ht="60">
+      <c r="B23" s="16" t="str">
         <f t="array" ref="B23">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B23)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B23))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2520,8 +2545,8 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B24" s="17" t="str">
+    <row r="24" spans="1:9" ht="75">
+      <c r="B24" s="16" t="str">
         <f t="array" ref="B24">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B24)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B24))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2538,8 +2563,8 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B25" s="17" t="str">
+    <row r="25" spans="1:9" ht="75">
+      <c r="B25" s="16" t="str">
         <f t="array" ref="B25">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B25)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B25))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2556,8 +2581,8 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B26" s="17" t="str">
+    <row r="26" spans="1:9" ht="75">
+      <c r="B26" s="16" t="str">
         <f t="array" ref="B26">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B26)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B26))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2574,8 +2599,8 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B27" s="17" t="str">
+    <row r="27" spans="1:9" ht="60">
+      <c r="B27" s="16" t="str">
         <f t="array" ref="B27">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B27)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B27))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2592,8 +2617,8 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="B28" s="17" t="str">
+    <row r="28" spans="1:9" ht="75">
+      <c r="B28" s="16" t="str">
         <f t="array" ref="B28">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B28)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B28))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2610,8 +2635,8 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B29" s="17" t="str">
+    <row r="29" spans="1:9" ht="60">
+      <c r="B29" s="16" t="str">
         <f t="array" ref="B29">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B29)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B29))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2628,8 +2653,8 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B30" s="17" t="str">
+    <row r="30" spans="1:9" ht="60">
+      <c r="B30" s="16" t="str">
         <f t="array" ref="B30">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B30)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B30))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2646,8 +2671,8 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B31" s="17" t="str">
+    <row r="31" spans="1:9" ht="60">
+      <c r="B31" s="16" t="str">
         <f t="array" ref="B31">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B31)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B31))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2664,8 +2689,8 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B32" s="17" t="str">
+    <row r="32" spans="1:9" ht="60">
+      <c r="B32" s="16" t="str">
         <f t="array" ref="B32">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B32)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B32))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2682,8 +2707,8 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B33" s="17" t="str">
+    <row r="33" spans="2:8" ht="45">
+      <c r="B33" s="16" t="str">
         <f t="array" ref="B33">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B33)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B33))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2700,8 +2725,8 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B34" s="17" t="str">
+    <row r="34" spans="2:8" ht="90">
+      <c r="B34" s="16" t="str">
         <f t="array" ref="B34">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B34)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B34))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2718,8 +2743,8 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B35" s="17" t="str">
+    <row r="35" spans="2:8" ht="75">
+      <c r="B35" s="16" t="str">
         <f t="array" ref="B35">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B35)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B35))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2736,8 +2761,8 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B36" s="17" t="str">
+    <row r="36" spans="2:8" ht="90">
+      <c r="B36" s="16" t="str">
         <f t="array" ref="B36">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B36)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B36))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2754,8 +2779,8 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B37" s="17" t="str">
+    <row r="37" spans="2:8" ht="60">
+      <c r="B37" s="16" t="str">
         <f t="array" ref="B37">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B37)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B37))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2772,8 +2797,8 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B38" s="17" t="str">
+    <row r="38" spans="2:8" ht="60">
+      <c r="B38" s="16" t="str">
         <f t="array" ref="B38">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B38)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B38))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2790,8 +2815,8 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B39" s="17" t="str">
+    <row r="39" spans="2:8" ht="60">
+      <c r="B39" s="16" t="str">
         <f t="array" ref="B39">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B39)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B39))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2808,8 +2833,8 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B40" s="17" t="str">
+    <row r="40" spans="2:8" ht="60">
+      <c r="B40" s="16" t="str">
         <f t="array" ref="B40">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B40)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B40))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2826,8 +2851,8 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="17" t="str">
+    <row r="41" spans="2:8">
+      <c r="B41" s="16" t="str">
         <f t="array" ref="B41">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B41)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B41))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2844,8 +2869,8 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="17" t="str">
+    <row r="42" spans="2:8">
+      <c r="B42" s="16" t="str">
         <f t="array" ref="B42">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B42)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B42))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2862,8 +2887,8 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="17" t="str">
+    <row r="43" spans="2:8">
+      <c r="B43" s="16" t="str">
         <f t="array" ref="B43">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B43)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B43))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2880,8 +2905,8 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="17" t="str">
+    <row r="44" spans="2:8">
+      <c r="B44" s="16" t="str">
         <f t="array" ref="B44">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B44)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B44))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2898,8 +2923,8 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="17" t="str">
+    <row r="45" spans="2:8">
+      <c r="B45" s="16" t="str">
         <f t="array" ref="B45">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B45)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B45))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2916,8 +2941,8 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="17" t="str">
+    <row r="46" spans="2:8">
+      <c r="B46" s="16" t="str">
         <f t="array" ref="B46">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B46)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B46))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2934,8 +2959,8 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="17" t="str">
+    <row r="47" spans="2:8">
+      <c r="B47" s="16" t="str">
         <f t="array" ref="B47">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B47)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B47))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2952,8 +2977,8 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="17" t="str">
+    <row r="48" spans="2:8">
+      <c r="B48" s="16" t="str">
         <f t="array" ref="B48">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B48)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B48))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2970,8 +2995,8 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="17" t="str">
+    <row r="49" spans="2:8">
+      <c r="B49" s="16" t="str">
         <f t="array" ref="B49">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B49)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B49))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -2988,8 +3013,8 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="17" t="str">
+    <row r="50" spans="2:8">
+      <c r="B50" s="16" t="str">
         <f t="array" ref="B50">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B50)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B50))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3006,8 +3031,8 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="17" t="str">
+    <row r="51" spans="2:8">
+      <c r="B51" s="16" t="str">
         <f t="array" ref="B51">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B51)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B51))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3024,8 +3049,8 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="17" t="str">
+    <row r="52" spans="2:8">
+      <c r="B52" s="16" t="str">
         <f t="array" ref="B52">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B52)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B52))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3042,8 +3067,8 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="17" t="str">
+    <row r="53" spans="2:8">
+      <c r="B53" s="16" t="str">
         <f t="array" ref="B53">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B53)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B53))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3060,8 +3085,8 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="17" t="str">
+    <row r="54" spans="2:8">
+      <c r="B54" s="16" t="str">
         <f t="array" ref="B54">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B54)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B54))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3078,8 +3103,8 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="17" t="str">
+    <row r="55" spans="2:8">
+      <c r="B55" s="16" t="str">
         <f t="array" ref="B55">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B55)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B55))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3096,8 +3121,8 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="17" t="str">
+    <row r="56" spans="2:8">
+      <c r="B56" s="16" t="str">
         <f t="array" ref="B56">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B56)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B56))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3114,8 +3139,8 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="17" t="str">
+    <row r="57" spans="2:8">
+      <c r="B57" s="16" t="str">
         <f t="array" ref="B57">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B57)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B57))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3132,8 +3157,8 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="17" t="str">
+    <row r="58" spans="2:8">
+      <c r="B58" s="16" t="str">
         <f t="array" ref="B58">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B58)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B58))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3150,8 +3175,8 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="17" t="str">
+    <row r="59" spans="2:8">
+      <c r="B59" s="16" t="str">
         <f t="array" ref="B59">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B59)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B59))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3168,8 +3193,8 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="17" t="str">
+    <row r="60" spans="2:8">
+      <c r="B60" s="16" t="str">
         <f t="array" ref="B60">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B60)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B60))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3186,8 +3211,8 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="17" t="str">
+    <row r="61" spans="2:8">
+      <c r="B61" s="16" t="str">
         <f t="array" ref="B61">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B61)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B61))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3204,8 +3229,8 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="17" t="str">
+    <row r="62" spans="2:8">
+      <c r="B62" s="16" t="str">
         <f t="array" ref="B62">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B62)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B62))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3222,8 +3247,8 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="17" t="str">
+    <row r="63" spans="2:8">
+      <c r="B63" s="16" t="str">
         <f t="array" ref="B63">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B63)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B63))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3240,8 +3265,8 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" s="17" t="str">
+    <row r="64" spans="2:8">
+      <c r="B64" s="16" t="str">
         <f t="array" ref="B64">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B64)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B64))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3258,8 +3283,8 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="17" t="str">
+    <row r="65" spans="2:8">
+      <c r="B65" s="16" t="str">
         <f t="array" ref="B65">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B65)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B65))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3276,8 +3301,8 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="17" t="str">
+    <row r="66" spans="2:8">
+      <c r="B66" s="16" t="str">
         <f t="array" ref="B66">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B66)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B66))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3294,8 +3319,8 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="17" t="str">
+    <row r="67" spans="2:8">
+      <c r="B67" s="16" t="str">
         <f t="array" ref="B67">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B67)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B67))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3312,8 +3337,8 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="17" t="str">
+    <row r="68" spans="2:8">
+      <c r="B68" s="16" t="str">
         <f t="array" ref="B68">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B68)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B68))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3330,8 +3355,8 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="17" t="str">
+    <row r="69" spans="2:8">
+      <c r="B69" s="16" t="str">
         <f t="array" ref="B69">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B69)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B69))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3348,8 +3373,8 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="17" t="str">
+    <row r="70" spans="2:8">
+      <c r="B70" s="16" t="str">
         <f t="array" ref="B70">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B70)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B70))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3366,8 +3391,8 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="17" t="str">
+    <row r="71" spans="2:8">
+      <c r="B71" s="16" t="str">
         <f t="array" ref="B71">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B71)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B71))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3384,8 +3409,8 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="17" t="str">
+    <row r="72" spans="2:8">
+      <c r="B72" s="16" t="str">
         <f t="array" ref="B72">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B72)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B72))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3402,8 +3427,8 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="17" t="str">
+    <row r="73" spans="2:8">
+      <c r="B73" s="16" t="str">
         <f t="array" ref="B73">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B73)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B73))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3420,8 +3445,8 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="17" t="str">
+    <row r="74" spans="2:8">
+      <c r="B74" s="16" t="str">
         <f t="array" ref="B74">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B74)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B74))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3438,8 +3463,8 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="17" t="str">
+    <row r="75" spans="2:8">
+      <c r="B75" s="16" t="str">
         <f t="array" ref="B75">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B75)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B75))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3456,8 +3481,8 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="17" t="str">
+    <row r="76" spans="2:8">
+      <c r="B76" s="16" t="str">
         <f t="array" ref="B76">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B76)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B76))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3474,8 +3499,8 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="17" t="str">
+    <row r="77" spans="2:8">
+      <c r="B77" s="16" t="str">
         <f t="array" ref="B77">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B77)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B77))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3492,8 +3517,8 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="17" t="str">
+    <row r="78" spans="2:8">
+      <c r="B78" s="16" t="str">
         <f t="array" ref="B78">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B78)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B78))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3510,8 +3535,8 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="17" t="str">
+    <row r="79" spans="2:8">
+      <c r="B79" s="16" t="str">
         <f t="array" ref="B79">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B79)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B79))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3528,8 +3553,8 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="17" t="str">
+    <row r="80" spans="2:8">
+      <c r="B80" s="16" t="str">
         <f t="array" ref="B80">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B80)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B80))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3546,8 +3571,8 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="17" t="str">
+    <row r="81" spans="2:8">
+      <c r="B81" s="16" t="str">
         <f t="array" ref="B81">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B81)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B81))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3564,8 +3589,8 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="17" t="str">
+    <row r="82" spans="2:8">
+      <c r="B82" s="16" t="str">
         <f t="array" ref="B82">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B82)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B82))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3582,8 +3607,8 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="17" t="str">
+    <row r="83" spans="2:8">
+      <c r="B83" s="16" t="str">
         <f t="array" ref="B83">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B83)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B83))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3600,8 +3625,8 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="17" t="str">
+    <row r="84" spans="2:8">
+      <c r="B84" s="16" t="str">
         <f t="array" ref="B84">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B84)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B84))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3618,8 +3643,8 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="17" t="str">
+    <row r="85" spans="2:8">
+      <c r="B85" s="16" t="str">
         <f t="array" ref="B85">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B85)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B85))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3636,8 +3661,8 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="17" t="str">
+    <row r="86" spans="2:8">
+      <c r="B86" s="16" t="str">
         <f t="array" ref="B86">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B86)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B86))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3654,8 +3679,8 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B87" s="17" t="str">
+    <row r="87" spans="2:8">
+      <c r="B87" s="16" t="str">
         <f t="array" ref="B87">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B87)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B87))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3672,8 +3697,8 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="17" t="str">
+    <row r="88" spans="2:8">
+      <c r="B88" s="16" t="str">
         <f t="array" ref="B88">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B88)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B88))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3690,8 +3715,8 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="17" t="str">
+    <row r="89" spans="2:8">
+      <c r="B89" s="16" t="str">
         <f t="array" ref="B89">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B89)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B89))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3708,8 +3733,8 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="17" t="str">
+    <row r="90" spans="2:8">
+      <c r="B90" s="16" t="str">
         <f t="array" ref="B90">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B90)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B90))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3726,8 +3751,8 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="17" t="str">
+    <row r="91" spans="2:8">
+      <c r="B91" s="16" t="str">
         <f t="array" ref="B91">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B91)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B91))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3744,8 +3769,8 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="17" t="str">
+    <row r="92" spans="2:8">
+      <c r="B92" s="16" t="str">
         <f t="array" ref="B92">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B92)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B92))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3762,8 +3787,8 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="17" t="str">
+    <row r="93" spans="2:8">
+      <c r="B93" s="16" t="str">
         <f t="array" ref="B93">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B93)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B93))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3780,8 +3805,8 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="17" t="str">
+    <row r="94" spans="2:8">
+      <c r="B94" s="16" t="str">
         <f t="array" ref="B94">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B94)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B94))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3798,8 +3823,8 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="17" t="str">
+    <row r="95" spans="2:8">
+      <c r="B95" s="16" t="str">
         <f t="array" ref="B95">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B95)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B95))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3816,8 +3841,8 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="17" t="str">
+    <row r="96" spans="2:8">
+      <c r="B96" s="16" t="str">
         <f t="array" ref="B96">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B96)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B96))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3834,8 +3859,8 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="17" t="str">
+    <row r="97" spans="2:8">
+      <c r="B97" s="16" t="str">
         <f t="array" ref="B97">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B97)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B97))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3852,8 +3877,8 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B98" s="17" t="str">
+    <row r="98" spans="2:8">
+      <c r="B98" s="16" t="str">
         <f t="array" ref="B98">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B98)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B98))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3870,8 +3895,8 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B99" s="17" t="str">
+    <row r="99" spans="2:8">
+      <c r="B99" s="16" t="str">
         <f t="array" ref="B99">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B99)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B99))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3888,8 +3913,8 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B100" s="17" t="str">
+    <row r="100" spans="2:8">
+      <c r="B100" s="16" t="str">
         <f t="array" ref="B100">IFERROR(INDEX(Atividade,SMALL(IF(Meta=$B$2,ROW(Atividade)-MIN(ROW(Atividade))+1),ROWS($B$3:B100)))&amp;" "&amp;CHAR(10)&amp;(INDEX(Resultado,SMALL(IF(Meta=$B$2,ROW(Resultado)-MIN(ROW(Resultado))+1),ROWS($B$3:B100))))&amp;CHAR(10),"")</f>
         <v/>
       </c>
@@ -3951,39 +3976,39 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="79.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="50.1" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="240" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="240">
       <c r="A3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="75">
       <c r="A5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>